<commit_message>
UPDATE robot.bd | version alpha 1
</commit_message>
<xml_diff>
--- a/resources/Planilla de facturacion - ACONCAGUA 02-2025.xlsx
+++ b/resources/Planilla de facturacion - ACONCAGUA 02-2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Escritorio\CLASE 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/58919b7dabedd3ac/Documents/git-and-github/RobotClase2/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EDA9E8-8F9F-4D41-828E-3AE33298F8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{37EDA9E8-8F9F-4D41-828E-3AE33298F8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CA3D957-68B4-44EA-8C6C-8B591284D7D2}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="1125" windowWidth="24510" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilla de Facturacion" sheetId="1" r:id="rId1"/>
@@ -73,18 +73,6 @@
     <t>Total Factura</t>
   </si>
   <si>
-    <t xml:space="preserve">00629                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsable Inscripto                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matias Pascual      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0003                                    </t>
-  </si>
-  <si>
     <t xml:space="preserve">BUTV 2H* Pago  cuota 30, 31 y  parte de </t>
   </si>
   <si>
@@ -94,12 +82,6 @@
     <t>AD2H</t>
   </si>
   <si>
-    <t xml:space="preserve">01927                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oscar Almaraz                    </t>
-  </si>
-  <si>
     <t>BUTL 10A* reemplazo echeq rechazado n° 4</t>
   </si>
   <si>
@@ -109,12 +91,6 @@
     <t>AD10A</t>
   </si>
   <si>
-    <t xml:space="preserve">06772                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsable Monotributo                 </t>
-  </si>
-  <si>
     <t>Emilio Rodríguez</t>
   </si>
   <si>
@@ -124,18 +100,12 @@
     <t>AL1</t>
   </si>
   <si>
-    <t xml:space="preserve">05992                                   </t>
-  </si>
-  <si>
     <t>Alejando Angilello</t>
   </si>
   <si>
     <t>BUTL L1* Pago saldo  cuota 7 de 12  Loca</t>
   </si>
   <si>
-    <t xml:space="preserve">08669                                  </t>
-  </si>
-  <si>
     <t>Sujeto Exento</t>
   </si>
   <si>
@@ -143,6 +113,36 @@
   </si>
   <si>
     <t>BUTL L1* Pago a cuenta cuota 8 de 12  Lo</t>
+  </si>
+  <si>
+    <t>00629</t>
+  </si>
+  <si>
+    <t>01927</t>
+  </si>
+  <si>
+    <t>06772</t>
+  </si>
+  <si>
+    <t>05992</t>
+  </si>
+  <si>
+    <t>08669</t>
+  </si>
+  <si>
+    <t>Responsable Monotributo</t>
+  </si>
+  <si>
+    <t>Responsable Inscripto</t>
+  </si>
+  <si>
+    <t>Matias Pascual</t>
+  </si>
+  <si>
+    <t>Oscar Almaraz</t>
+  </si>
+  <si>
+    <t>0003</t>
   </si>
 </sst>
 </file>
@@ -150,10 +150,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#0.00"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#0.00"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -373,12 +373,12 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -399,24 +399,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -426,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Millares 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Millares 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Millares 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -746,30 +746,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="12" customWidth="1"/>
     <col min="8" max="8" width="10" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="18" customWidth="1"/>
-    <col min="11" max="12" width="14.140625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="18" customWidth="1"/>
-    <col min="15" max="16" width="11.42578125" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="12"/>
+    <col min="9" max="9" width="11.44140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="18" customWidth="1"/>
+    <col min="11" max="12" width="14.109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" style="18" customWidth="1"/>
+    <col min="15" max="16" width="11.44140625" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="11.44140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="N1" s="31"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -811,7 +811,7 @@
       <c r="N2" s="34"/>
       <c r="O2" s="15"/>
     </row>
-    <row r="3" spans="1:15" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -854,30 +854,30 @@
       </c>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D4" s="11">
         <v>45716</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3">
         <v>0.105</v>
@@ -897,30 +897,30 @@
       </c>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D5" s="11">
         <v>45716</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G5" s="22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3">
         <v>0.105</v>
@@ -940,30 +940,30 @@
       </c>
       <c r="O5" s="15"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D6" s="11">
         <v>45716</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I6" s="3">
         <v>0.21</v>
@@ -983,30 +983,30 @@
       </c>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D7" s="11">
         <v>45716</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I7" s="3">
         <v>0.21</v>
@@ -1026,30 +1026,30 @@
       </c>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D8" s="11">
         <v>45716</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I8" s="3">
         <v>0.21</v>

</xml_diff>